<commit_message>
:sparkles: Bundle rm_sumrow() and rm_sumcol() to rebel()
</commit_message>
<xml_diff>
--- a/tests/testthat/sumcol_contami.xlsx
+++ b/tests/testthat/sumcol_contami.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="17620" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="36">
   <si>
     <t>A1</t>
   </si>
@@ -452,7 +453,7 @@
   <dimension ref="A1:H30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="G2" sqref="G2:G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -488,6 +489,859 @@
         <v>1</v>
       </c>
       <c r="B2">
+        <v>212</v>
+      </c>
+      <c r="C2">
+        <v>242</v>
+      </c>
+      <c r="D2">
+        <f>SUM(B2:C2)</f>
+        <v>454</v>
+      </c>
+      <c r="E2">
+        <v>302</v>
+      </c>
+      <c r="F2">
+        <v>332</v>
+      </c>
+      <c r="G2">
+        <f>SUM(E2:F2)</f>
+        <v>634</v>
+      </c>
+      <c r="H2">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>213</v>
+      </c>
+      <c r="C3">
+        <v>243</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D30" si="0">SUM(B3:C3)</f>
+        <v>456</v>
+      </c>
+      <c r="E3">
+        <v>303</v>
+      </c>
+      <c r="F3">
+        <v>333</v>
+      </c>
+      <c r="G3">
+        <f t="shared" ref="G3:G30" si="1">SUM(E3:F3)</f>
+        <v>636</v>
+      </c>
+      <c r="H3">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>214</v>
+      </c>
+      <c r="C4">
+        <v>244</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>458</v>
+      </c>
+      <c r="E4">
+        <v>304</v>
+      </c>
+      <c r="F4">
+        <v>334</v>
+      </c>
+      <c r="G4">
+        <f t="shared" si="1"/>
+        <v>638</v>
+      </c>
+      <c r="H4">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>215</v>
+      </c>
+      <c r="C5">
+        <v>245</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>460</v>
+      </c>
+      <c r="E5">
+        <v>305</v>
+      </c>
+      <c r="F5">
+        <v>335</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="1"/>
+        <v>640</v>
+      </c>
+      <c r="H5">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>216</v>
+      </c>
+      <c r="C6">
+        <v>246</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>462</v>
+      </c>
+      <c r="E6">
+        <v>306</v>
+      </c>
+      <c r="F6">
+        <v>336</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="1"/>
+        <v>642</v>
+      </c>
+      <c r="H6">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>217</v>
+      </c>
+      <c r="C7">
+        <v>247</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>464</v>
+      </c>
+      <c r="E7">
+        <v>307</v>
+      </c>
+      <c r="F7">
+        <v>337</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="1"/>
+        <v>644</v>
+      </c>
+      <c r="H7">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>218</v>
+      </c>
+      <c r="C8">
+        <v>248</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>466</v>
+      </c>
+      <c r="E8">
+        <v>308</v>
+      </c>
+      <c r="F8">
+        <v>338</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="1"/>
+        <v>646</v>
+      </c>
+      <c r="H8">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>219</v>
+      </c>
+      <c r="C9">
+        <v>249</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>468</v>
+      </c>
+      <c r="E9">
+        <v>309</v>
+      </c>
+      <c r="F9">
+        <v>339</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="1"/>
+        <v>648</v>
+      </c>
+      <c r="H9">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>220</v>
+      </c>
+      <c r="C10">
+        <v>250</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>470</v>
+      </c>
+      <c r="E10">
+        <v>310</v>
+      </c>
+      <c r="F10">
+        <v>340</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="1"/>
+        <v>650</v>
+      </c>
+      <c r="H10">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>221</v>
+      </c>
+      <c r="C11">
+        <v>251</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>472</v>
+      </c>
+      <c r="E11">
+        <v>311</v>
+      </c>
+      <c r="F11">
+        <v>341</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="1"/>
+        <v>652</v>
+      </c>
+      <c r="H11">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>222</v>
+      </c>
+      <c r="C12">
+        <v>252</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>474</v>
+      </c>
+      <c r="E12">
+        <v>312</v>
+      </c>
+      <c r="F12">
+        <v>342</v>
+      </c>
+      <c r="G12">
+        <f t="shared" si="1"/>
+        <v>654</v>
+      </c>
+      <c r="H12">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>223</v>
+      </c>
+      <c r="C13">
+        <v>253</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>476</v>
+      </c>
+      <c r="E13">
+        <v>313</v>
+      </c>
+      <c r="F13">
+        <v>343</v>
+      </c>
+      <c r="G13">
+        <f t="shared" si="1"/>
+        <v>656</v>
+      </c>
+      <c r="H13">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>224</v>
+      </c>
+      <c r="C14">
+        <v>254</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>478</v>
+      </c>
+      <c r="E14">
+        <v>314</v>
+      </c>
+      <c r="F14">
+        <v>344</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="1"/>
+        <v>658</v>
+      </c>
+      <c r="H14">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>225</v>
+      </c>
+      <c r="C15">
+        <v>255</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>480</v>
+      </c>
+      <c r="E15">
+        <v>315</v>
+      </c>
+      <c r="F15">
+        <v>345</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>660</v>
+      </c>
+      <c r="H15">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>226</v>
+      </c>
+      <c r="C16">
+        <v>256</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>482</v>
+      </c>
+      <c r="E16">
+        <v>316</v>
+      </c>
+      <c r="F16">
+        <v>346</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="1"/>
+        <v>662</v>
+      </c>
+      <c r="H16">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>16</v>
+      </c>
+      <c r="B17">
+        <v>227</v>
+      </c>
+      <c r="C17">
+        <v>257</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>484</v>
+      </c>
+      <c r="E17">
+        <v>317</v>
+      </c>
+      <c r="F17">
+        <v>347</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="1"/>
+        <v>664</v>
+      </c>
+      <c r="H17">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18">
+        <v>228</v>
+      </c>
+      <c r="C18">
+        <v>258</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>486</v>
+      </c>
+      <c r="E18">
+        <v>318</v>
+      </c>
+      <c r="F18">
+        <v>348</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="1"/>
+        <v>666</v>
+      </c>
+      <c r="H18">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A19" t="s">
+        <v>18</v>
+      </c>
+      <c r="B19">
+        <v>229</v>
+      </c>
+      <c r="C19">
+        <v>259</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>488</v>
+      </c>
+      <c r="E19">
+        <v>319</v>
+      </c>
+      <c r="F19">
+        <v>349</v>
+      </c>
+      <c r="G19">
+        <f t="shared" si="1"/>
+        <v>668</v>
+      </c>
+      <c r="H19">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20">
+        <v>230</v>
+      </c>
+      <c r="C20">
+        <v>260</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>490</v>
+      </c>
+      <c r="E20">
+        <v>320</v>
+      </c>
+      <c r="F20">
+        <v>350</v>
+      </c>
+      <c r="G20">
+        <f t="shared" si="1"/>
+        <v>670</v>
+      </c>
+      <c r="H20">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21">
+        <v>231</v>
+      </c>
+      <c r="C21">
+        <v>261</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>492</v>
+      </c>
+      <c r="E21">
+        <v>321</v>
+      </c>
+      <c r="F21">
+        <v>351</v>
+      </c>
+      <c r="G21">
+        <f t="shared" si="1"/>
+        <v>672</v>
+      </c>
+      <c r="H21">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>21</v>
+      </c>
+      <c r="B22">
+        <v>232</v>
+      </c>
+      <c r="C22">
+        <v>262</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>494</v>
+      </c>
+      <c r="E22">
+        <v>322</v>
+      </c>
+      <c r="F22">
+        <v>352</v>
+      </c>
+      <c r="G22">
+        <f t="shared" si="1"/>
+        <v>674</v>
+      </c>
+      <c r="H22">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>22</v>
+      </c>
+      <c r="B23">
+        <v>233</v>
+      </c>
+      <c r="C23">
+        <v>263</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>496</v>
+      </c>
+      <c r="E23">
+        <v>323</v>
+      </c>
+      <c r="F23">
+        <v>353</v>
+      </c>
+      <c r="G23">
+        <f t="shared" si="1"/>
+        <v>676</v>
+      </c>
+      <c r="H23">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>234</v>
+      </c>
+      <c r="C24">
+        <v>264</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>498</v>
+      </c>
+      <c r="E24">
+        <v>324</v>
+      </c>
+      <c r="F24">
+        <v>354</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="1"/>
+        <v>678</v>
+      </c>
+      <c r="H24">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
+        <v>235</v>
+      </c>
+      <c r="C25">
+        <v>265</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+      <c r="E25">
+        <v>325</v>
+      </c>
+      <c r="F25">
+        <v>355</v>
+      </c>
+      <c r="G25">
+        <f t="shared" si="1"/>
+        <v>680</v>
+      </c>
+      <c r="H25">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26">
+        <v>236</v>
+      </c>
+      <c r="C26">
+        <v>266</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>502</v>
+      </c>
+      <c r="E26">
+        <v>326</v>
+      </c>
+      <c r="F26">
+        <v>356</v>
+      </c>
+      <c r="G26">
+        <f t="shared" si="1"/>
+        <v>682</v>
+      </c>
+      <c r="H26">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27">
+        <v>237</v>
+      </c>
+      <c r="C27">
+        <v>267</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>504</v>
+      </c>
+      <c r="E27">
+        <v>327</v>
+      </c>
+      <c r="F27">
+        <v>357</v>
+      </c>
+      <c r="G27">
+        <f t="shared" si="1"/>
+        <v>684</v>
+      </c>
+      <c r="H27">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28">
+        <v>238</v>
+      </c>
+      <c r="C28">
+        <v>268</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>506</v>
+      </c>
+      <c r="E28">
+        <v>328</v>
+      </c>
+      <c r="F28">
+        <v>358</v>
+      </c>
+      <c r="G28">
+        <f t="shared" si="1"/>
+        <v>686</v>
+      </c>
+      <c r="H28">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29">
+        <v>239</v>
+      </c>
+      <c r="C29">
+        <v>269</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>508</v>
+      </c>
+      <c r="E29">
+        <v>329</v>
+      </c>
+      <c r="F29">
+        <v>359</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="1"/>
+        <v>688</v>
+      </c>
+      <c r="H29">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30">
+        <v>240</v>
+      </c>
+      <c r="C30">
+        <v>270</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>510</v>
+      </c>
+      <c r="E30">
+        <v>330</v>
+      </c>
+      <c r="F30">
+        <v>360</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="1"/>
+        <v>690</v>
+      </c>
+      <c r="H30">
+        <v>420</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H30"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2:D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" t="s">
+        <v>35</v>
+      </c>
+      <c r="H1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>2</v>
       </c>
       <c r="C2">

</xml_diff>